<commit_message>
update province figure value error
</commit_message>
<xml_diff>
--- a/outcome/appendix/Table S3.xlsx
+++ b/outcome/appendix/Table S3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">province</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tibet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Xinjiang</t>
@@ -1056,16 +1053,16 @@
         <v>39448</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44166</v>
+        <v>45261</v>
       </c>
       <c r="D30" t="n">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="n">
-        <v>3744</v>
+        <v>4608</v>
       </c>
     </row>
     <row r="31">
@@ -1076,16 +1073,16 @@
         <v>39448</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>45261</v>
+        <v>44166</v>
       </c>
       <c r="D31" t="n">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
       </c>
       <c r="F31" t="n">
-        <v>4608</v>
+        <v>3744</v>
       </c>
     </row>
     <row r="32">
@@ -1096,35 +1093,15 @@
         <v>39448</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44166</v>
+        <v>45261</v>
       </c>
       <c r="D32" t="n">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>3744</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>39448</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>45261</v>
-      </c>
-      <c r="D33" t="n">
-        <v>192</v>
-      </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" t="n">
         <v>4608</v>
       </c>
     </row>

</xml_diff>